<commit_message>
Modification of selection criteria for MS cohort
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_DU_selection_criteria_from_SAP1_MS_cohort_to_DU_MS_cohort.xlsx
+++ b/i_codebooks/D3_DU_selection_criteria_from_SAP1_MS_cohort_to_DU_MS_cohort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lol\Documents\DP3-MS-SLE\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9F1280-EA4B-4FB5-B2F2-4BFB25DC929A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DCC429-2F34-4E78-A526-C5DF79922D25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Parameters" sheetId="3" r:id="rId3"/>
     <sheet name="Example" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mhzNGBeK9861EYEtgLjD+CXFeX/VQ=="/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>medatata_name</t>
   </si>
@@ -134,15 +134,7 @@
     <t>Rule</t>
   </si>
   <si>
-    <t>women_diagnosed_outside_childbearing_age</t>
-  </si>
-  <si>
     <t>women_with_less_than_1_year_fup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 = outside of childbearing age
-1 = otherwise
-</t>
   </si>
   <si>
     <t xml:space="preserve">0 = less than year of follow up at diagnosis date
@@ -156,9 +148,6 @@
     <t>excludes persons who are  never positive for MS_chosen during their study period, that is, who are not stored in D3_SAP1_MS-COHORT</t>
   </si>
   <si>
-    <t>excludes persons which are &lt; 15 years old and &gt; 50 at D3_SAP1_MS-COHORT/date_MS</t>
-  </si>
-  <si>
     <t>excludes women who are diagnosed &lt;1 year before D3_SAP1_MS-COHORT/cohort_exit_date</t>
   </si>
   <si>
@@ -170,16 +159,40 @@
   <si>
     <t xml:space="preserve">test </t>
   </si>
+  <si>
+    <t xml:space="preserve">0 = after childbearing age (&gt;49)
+1 = otherwise
+</t>
+  </si>
+  <si>
+    <t>women_diagnosed_after_childbearing_age</t>
+  </si>
+  <si>
+    <t>excludes persons which are &gt; 50  years old at D3_SAP1_MS-COHORT/date_MS</t>
+  </si>
+  <si>
+    <t>should be 0</t>
+  </si>
+  <si>
+    <t>Only for datasources with complete cohort of Women of childbearing age (Norway, Wales and Emilia Romania)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -390,64 +403,68 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9149,10 +9166,10 @@
   <dimension ref="A1:K996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9189,7 +9206,7 @@
         <v>10</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>30</v>
@@ -9219,7 +9236,7 @@
       </c>
       <c r="E2" s="8"/>
       <c r="H2" s="21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -9227,7 +9244,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -9236,48 +9253,54 @@
         <v>29</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="I4" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>46</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>